<commit_message>
practicing writing to python
doesn't seem to be working still
</commit_message>
<xml_diff>
--- a/LoveCraftsScrape.xlsx
+++ b/LoveCraftsScrape.xlsx
@@ -14,12 +14,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>yarn info</t>
   </si>
   <si>
     <t>pricing</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        50% Wool 50% Acrylic, 180m (197yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 88m (96yds)/50g (1.8oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 880m (962yds)/500g (17.6oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 200m (219yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 166m (182yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 90m (98yds)/50g (1.8oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 900m (984yds)/500g (17.6oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 440m (481yds)/250g (8.8oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        50% Wool 25% Alpaca 25% Viscose, 87m (95yds)/50g (1.8oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 100m (109yds)/50g (1.8oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 180m (197yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        50% Wool 50% Acrylic, 500g (17.6oz)
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        35% Wool 20% Acrylic 20% Polyamide 25% Viscose, 300m (328yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        100% Wool, 137m (150yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        96% Wool 4% Viscose, 166m (182yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+        80% Wool 20% Polyamide, 199m (218yds)/100g (3.5oz), Aran
+      &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="product-card__subtitle"&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £7.00
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £8.49
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £9.99
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £7.49
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £9.49
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £6.95
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £4.99
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £3.49
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £8.70
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £6.90
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £4.49
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £10.99
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £12.99
+    &lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+      £6.25
+    &lt;/span&gt;&lt;/span&gt;</t>
   </si>
 </sst>
 </file>
@@ -377,18 +531,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
splitted the lists and made it more efficient
</commit_message>
<xml_diff>
--- a/LoveCraftsScrape.xlsx
+++ b/LoveCraftsScrape.xlsx
@@ -14,166 +14,148 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
-  <si>
-    <t>yarn info</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+  <si>
+    <t>fibre</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
   <si>
     <t>pricing</t>
   </si>
   <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        50% Wool 50% Acrylic, 180m (197yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 88m (96yds)/50g (1.8oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 880m (962yds)/500g (17.6oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 200m (219yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 166m (182yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 90m (98yds)/50g (1.8oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 900m (984yds)/500g (17.6oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 440m (481yds)/250g (8.8oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        50% Wool 25% Alpaca 25% Viscose, 87m (95yds)/50g (1.8oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 100m (109yds)/50g (1.8oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 180m (197yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        50% Wool 50% Acrylic, 500g (17.6oz)
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        35% Wool 20% Acrylic 20% Polyamide 25% Viscose, 300m (328yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        100% Wool, 137m (150yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        96% Wool 4% Viscose, 166m (182yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-        80% Wool 20% Polyamide, 199m (218yds)/100g (3.5oz), Aran
-      &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="product-card__subtitle"&gt;
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    <t>50% Wool 50% Acrylic</t>
+  </si>
+  <si>
+    <t>100% Wool</t>
+  </si>
+  <si>
+    <t>50% Wool 25% Alpaca 25% Viscose</t>
+  </si>
+  <si>
+    <t>35% Wool 20% Acrylic 20% Polyamide 25% Viscose</t>
+  </si>
+  <si>
+    <t>96% Wool 4% Viscose</t>
+  </si>
+  <si>
+    <t>80% Wool 20% Polyamide</t>
+  </si>
+  <si>
+    <t>180m (197yds)/100g (3.5oz)</t>
+  </si>
+  <si>
+    <t>88m (96yds)/50g (1.8oz)</t>
+  </si>
+  <si>
+    <t>880m (962yds)/500g (17.6oz)</t>
+  </si>
+  <si>
+    <t>200m (219yds)/100g (3.5oz)</t>
+  </si>
+  <si>
+    <t>166m (182yds)/100g (3.5oz)</t>
+  </si>
+  <si>
+    <t>90m (98yds)/50g (1.8oz)</t>
+  </si>
+  <si>
+    <t>900m (984yds)/500g (17.6oz)</t>
+  </si>
+  <si>
+    <t>440m (481yds)/250g (8.8oz)</t>
+  </si>
+  <si>
+    <t>87m (95yds)/50g (1.8oz)</t>
+  </si>
+  <si>
+    <t>100m (109yds)/50g (1.8oz)</t>
+  </si>
+  <si>
+    <t>300m (328yds)/100g (3.5oz)</t>
+  </si>
+  <si>
+    <t>137m (150yds)/100g (3.5oz)</t>
+  </si>
+  <si>
+    <t>199m (218yds)/100g (3.5oz)</t>
+  </si>
+  <si>
+    <t>Aran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £7.00
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £8.49
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £9.99
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £7.49
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £9.49
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £6.95
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £4.99
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £3.49
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £8.70
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £6.90
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £4.49
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £10.99
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £12.99
-    &lt;/span&gt;&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span class="lc-price__regular" data-v-27ab4212=""&gt;&lt;span data-v-27ab4212=""&gt;
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
       £6.25
-    &lt;/span&gt;&lt;/span&gt;</t>
+    </t>
   </si>
 </sst>
 </file>
@@ -531,54 +513,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -586,172 +592,234 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in the name of different yarns
basically the completed version without the math element to refer back to for when i mess up the math element
</commit_message>
<xml_diff>
--- a/LoveCraftsScrape.xlsx
+++ b/LoveCraftsScrape.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+  <si>
+    <t>name</t>
+  </si>
   <si>
     <t>fibre</t>
   </si>
@@ -28,6 +31,57 @@
     <t>pricing</t>
   </si>
   <si>
+    <t>Paintbox Yarns Wool Mix Aran</t>
+  </si>
+  <si>
+    <t>Debbie Bliss Donegal Luxury Tweed Aran</t>
+  </si>
+  <si>
+    <t>Debbie Bliss Donegal Luxury Tweed Aran 10 Ball Value Pack</t>
+  </si>
+  <si>
+    <t>Cascade 220</t>
+  </si>
+  <si>
+    <t>West Yorkshire Spinners The Croft</t>
+  </si>
+  <si>
+    <t>Debbie Bliss British Wool Aran</t>
+  </si>
+  <si>
+    <t>Debbie Bliss British Wool Aran 10 Ball Value Pack</t>
+  </si>
+  <si>
+    <t>Debbie Bliss Donegal Luxury Tweed Aran 5 Ball Value Pack</t>
+  </si>
+  <si>
+    <t>West Yorkshire Spinners Jacobs Aran</t>
+  </si>
+  <si>
+    <t>Rowan Felted Tweed Aran</t>
+  </si>
+  <si>
+    <t>West Yorkshire Spinners ColourLab Aran</t>
+  </si>
+  <si>
+    <t>Noro Kureyon</t>
+  </si>
+  <si>
+    <t>King Cole Wool Aran</t>
+  </si>
+  <si>
+    <t>King Cole Forest Aran</t>
+  </si>
+  <si>
+    <t>Cascade Yarns 220 Superwash Aran Wave</t>
+  </si>
+  <si>
+    <t>West Yorkshire Spinners ColourLab Aran Tweed</t>
+  </si>
+  <si>
+    <t>Novita 7 Veljestä</t>
+  </si>
+  <si>
     <t>50% Wool 50% Acrylic</t>
   </si>
   <si>
@@ -88,74 +142,46 @@
     <t>Aran</t>
   </si>
   <si>
-    <t xml:space="preserve">
-      £7.00
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £8.49
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £9.99
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £7.49
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £9.49
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £6.95
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £4.99
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £3.49
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £8.70
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £6.90
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £4.49
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £10.99
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £12.99
-    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-      £6.25
-    </t>
+    <t>£7.00</t>
+  </si>
+  <si>
+    <t>£8.49</t>
+  </si>
+  <si>
+    <t>£9.99</t>
+  </si>
+  <si>
+    <t>£7.49</t>
+  </si>
+  <si>
+    <t>£9.49</t>
+  </si>
+  <si>
+    <t>£6.95</t>
+  </si>
+  <si>
+    <t>£4.99</t>
+  </si>
+  <si>
+    <t>£3.49</t>
+  </si>
+  <si>
+    <t>£8.70</t>
+  </si>
+  <si>
+    <t>£6.90</t>
+  </si>
+  <si>
+    <t>£4.49</t>
+  </si>
+  <si>
+    <t>£10.99</t>
+  </si>
+  <si>
+    <t>£12.99</t>
+  </si>
+  <si>
+    <t>£6.25</t>
   </si>
 </sst>
 </file>
@@ -513,13 +539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,294 +558,348 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>